<commit_message>
Apply corrections to verifications matrix
</commit_message>
<xml_diff>
--- a/ExcelTables/Matrices para MML.xlsx
+++ b/ExcelTables/Matrices para MML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanb\OneDrive\Documentos\GitHub\GerenciaProyectos\ExcelTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A055492-0DA5-4A18-AEEC-F942DE039011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF918153-CB60-471B-94AB-FE08A6958264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores y metas inter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="146">
   <si>
     <t>NIVEL</t>
   </si>
@@ -410,15 +410,9 @@
     <t>Anual</t>
   </si>
   <si>
-    <t>Alcaldía Local</t>
-  </si>
-  <si>
     <t>Consulta en las bases de datos del sistema, mediante reportes automáticos o consultas que miden el tiempo entre la radicación y la aprobación.</t>
   </si>
   <si>
-    <t>(Cuantitativo) Análisi cuantitativo del aumento de la cantidad de licencias procesadas mensualmente antes y después de la implementación del sistema</t>
-  </si>
-  <si>
     <t>Mensual</t>
   </si>
   <si>
@@ -440,19 +434,10 @@
     <t>Revisión documental de las actas de recepción y verificación física del inventario para confirmar ubicación y número de serie.</t>
   </si>
   <si>
-    <t>(Cuantitativo) Calculo del porcentaje de equipos instalados.</t>
-  </si>
-  <si>
     <t>Revisión documental de las listas de asistencia y los registros de las calificaciones obtenidas en las pruebas finales.</t>
   </si>
   <si>
-    <t>(Cuantitativo) Calculo del porcentaje de asistencia y aprobación.</t>
-  </si>
-  <si>
     <t>Trimestral</t>
-  </si>
-  <si>
-    <t>Talento Humano</t>
   </si>
   <si>
     <t>Documento final</t>
@@ -552,6 +537,24 @@
   <si>
     <t>Revisión de documentos de
 arrendamiento</t>
+  </si>
+  <si>
+    <t>DANE</t>
+  </si>
+  <si>
+    <t>(Cuantitativo) Análisis cuantitativo del aumento de la cantidad de licencias procesadas mensualmente antes y después de la implementación del sistema</t>
+  </si>
+  <si>
+    <t>(Cuantitativo) Cálculo del porcentaje de equipos instalados.</t>
+  </si>
+  <si>
+    <t>Ingenieros de Sistemas</t>
+  </si>
+  <si>
+    <t>(Cuantitativo) Cálculo del porcentaje de asistencia y aprobación.</t>
+  </si>
+  <si>
+    <t>Jefe de Área</t>
   </si>
 </sst>
 </file>
@@ -1525,7 +1528,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1795,6 +1798,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1807,40 +1819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1859,7 +1838,22 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2661,6 +2655,50 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>11683</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1724026</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>391595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AFA9487-1BF6-438E-B0C3-478FA1E677C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4336033" y="4688205"/>
+          <a:ext cx="1712343" cy="284915"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3314,7 +3352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AG994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
@@ -9960,8 +9998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9971,36 +10009,38 @@
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="26" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="26" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="110" t="s">
+      <c r="E4" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="110" t="s">
+      <c r="F4" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
     </row>
     <row r="5" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
       <c r="F5" s="64" t="s">
         <v>40</v>
       </c>
@@ -10018,10 +10058,10 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="112" t="s">
+      <c r="D6" s="105" t="s">
         <v>98</v>
       </c>
       <c r="E6" s="65"/>
@@ -10032,8 +10072,8 @@
       <c r="J6" s="65"/>
     </row>
     <row r="7" spans="3:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="111"/>
-      <c r="D7" s="112"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="105"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
       <c r="G7" s="65"/>
@@ -10042,8 +10082,8 @@
       <c r="J7" s="65"/>
     </row>
     <row r="8" spans="3:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="111"/>
-      <c r="D8" s="112"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
       <c r="E8" s="65"/>
       <c r="F8" s="66"/>
       <c r="G8" s="65"/>
@@ -10088,7 +10128,7 @@
         <v>101</v>
       </c>
       <c r="J10" s="62" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="3:10" ht="128.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10105,160 +10145,170 @@
         <v>79</v>
       </c>
       <c r="G11" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="I11" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="J11" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="I11" s="62" t="s">
+    </row>
+    <row r="12" spans="3:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="108" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="62" t="s">
+      <c r="D12" s="106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="109" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="12" spans="3:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="105" t="s">
+      <c r="H12" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="103" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="107" t="s">
+      <c r="I12" s="106" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="106" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="108"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+    </row>
+    <row r="14" spans="3:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="108"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="106"/>
+      <c r="J14" s="106"/>
+    </row>
+    <row r="15" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="108"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="106" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="106" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" s="106" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="106" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="108"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="103" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="103" t="s">
-        <v>108</v>
-      </c>
-      <c r="H12" s="103" t="s">
-        <v>109</v>
-      </c>
-      <c r="I12" s="103" t="s">
-        <v>105</v>
-      </c>
-      <c r="J12" s="103" t="s">
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="106"/>
+    </row>
+    <row r="17" spans="3:10" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="108"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
+    </row>
+    <row r="18" spans="3:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="108"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="106" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="106" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="3:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="105"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
-    </row>
-    <row r="14" spans="3:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="105"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="108"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-    </row>
-    <row r="15" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="105"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-    </row>
-    <row r="16" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="105"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="106" t="s">
+      <c r="H18" s="106" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" s="106" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="108"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="103" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="103" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" s="103" t="s">
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
+    </row>
+    <row r="20" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="108"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="106"/>
+    </row>
+    <row r="21" spans="3:10" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="108"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="I16" s="103" t="s">
-        <v>105</v>
-      </c>
-      <c r="J16" s="103" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="105"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="103"/>
-    </row>
-    <row r="18" spans="3:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="105"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
-    </row>
-    <row r="19" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="105"/>
-      <c r="D19" s="103"/>
-      <c r="E19" s="106" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="103" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="103" t="s">
+      <c r="H21" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="103" t="s">
+      <c r="I21" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="103" t="s">
+      <c r="J21" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="103" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="105"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="103"/>
-      <c r="I20" s="103"/>
-      <c r="J20" s="103"/>
-    </row>
-    <row r="21" spans="3:10" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="105"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="103"/>
-      <c r="J21" s="103"/>
-    </row>
-    <row r="22" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="104" t="s">
+    </row>
+    <row r="22" spans="3:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="107" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="71" t="s">
@@ -10267,72 +10317,72 @@
       <c r="E22" s="72">
         <v>695000000</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" s="73" t="s">
+      <c r="F22" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="62" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="104"/>
+    </row>
+    <row r="23" spans="3:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="107"/>
       <c r="D23" s="71" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="72">
         <v>5000000</v>
       </c>
-      <c r="F23" s="62" t="s">
-        <v>86</v>
+      <c r="F23" s="73" t="s">
+        <v>87</v>
       </c>
       <c r="G23" s="62" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H23" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I23" s="62" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J23" s="62" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="104"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="107"/>
       <c r="D24" s="29" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="74">
         <v>2000000</v>
       </c>
-      <c r="F24" s="73" t="s">
-        <v>87</v>
+      <c r="F24" s="62" t="s">
+        <v>88</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H24" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I24" s="62" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="104"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="107"/>
       <c r="D25" s="29" t="s">
         <v>27</v>
       </c>
@@ -10340,23 +10390,23 @@
         <v>6000000</v>
       </c>
       <c r="F25" s="62" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G25" s="62" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H25" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I25" s="62" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J25" s="62" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="104"/>
+    <row r="26" spans="3:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="107"/>
       <c r="D26" s="29" t="s">
         <v>28</v>
       </c>
@@ -10364,23 +10414,23 @@
         <v>12000000</v>
       </c>
       <c r="F26" s="62" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G26" s="62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H26" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I26" s="62" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="104"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="107"/>
       <c r="D27" s="29" t="s">
         <v>29</v>
       </c>
@@ -10388,23 +10438,23 @@
         <v>12000000</v>
       </c>
       <c r="F27" s="62" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G27" s="62" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H27" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I27" s="62" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J27" s="62" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="104"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="107"/>
       <c r="D28" s="29" t="s">
         <v>30</v>
       </c>
@@ -10412,23 +10462,23 @@
         <v>12000000</v>
       </c>
       <c r="F28" s="62" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G28" s="62" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H28" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I28" s="62" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="J28" s="62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="104"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="107"/>
       <c r="D29" s="29" t="s">
         <v>31</v>
       </c>
@@ -10439,20 +10489,20 @@
         <v>92</v>
       </c>
       <c r="G29" s="62" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H29" s="62" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="I29" s="62" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J29" s="62" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="104"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="107"/>
       <c r="D30" s="62" t="s">
         <v>32</v>
       </c>
@@ -10460,23 +10510,23 @@
         <v>10000000</v>
       </c>
       <c r="F30" s="62" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G30" s="62" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H30" s="62" t="s">
         <v>46</v>
       </c>
       <c r="I30" s="62" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="J30" s="62" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="104"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="107"/>
       <c r="D31" s="62" t="s">
         <v>33</v>
       </c>
@@ -10484,23 +10534,23 @@
         <v>480000000</v>
       </c>
       <c r="F31" s="62" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G31" s="62" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H31" s="62" t="s">
         <v>46</v>
       </c>
       <c r="I31" s="62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J31" s="62" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="104"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="107"/>
       <c r="D32" s="62" t="s">
         <v>34</v>
       </c>
@@ -10508,23 +10558,23 @@
         <v>60000000</v>
       </c>
       <c r="F32" s="62" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G32" s="62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H32" s="62" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="I32" s="62" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="104"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="107"/>
       <c r="D33" s="62" t="s">
         <v>35</v>
       </c>
@@ -10535,20 +10585,20 @@
         <v>95</v>
       </c>
       <c r="G33" s="62" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H33" s="62" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="I33" s="62" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="J33" s="62" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="104"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="107"/>
       <c r="D34" s="62" t="s">
         <v>36</v>
       </c>
@@ -10556,23 +10606,23 @@
         <v>5000000</v>
       </c>
       <c r="F34" s="62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G34" s="62" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H34" s="62" t="s">
         <v>46</v>
       </c>
       <c r="I34" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="J34" s="62" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="104"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="107"/>
       <c r="D35" s="62" t="s">
         <v>37</v>
       </c>
@@ -10580,23 +10630,23 @@
         <v>25000000</v>
       </c>
       <c r="F35" s="62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G35" s="62" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H35" s="62" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="I35" s="62" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="J35" s="62" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="104"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="107"/>
       <c r="D36" s="62" t="s">
         <v>38</v>
       </c>
@@ -10607,16 +10657,16 @@
         <v>97</v>
       </c>
       <c r="G36" s="62" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H36" s="62" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I36" s="62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J36" s="62" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11585,37 +11635,37 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="C22:C36"/>
+    <mergeCell ref="D12:D21"/>
+    <mergeCell ref="C12:C21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="F18:F20"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="C22:C36"/>
-    <mergeCell ref="D12:D21"/>
-    <mergeCell ref="C12:C21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{19781335-1720-47F8-9FA4-422E5A6BE884}"/>
-    <hyperlink ref="F11" r:id="rId2" xr:uid="{EC3CF793-07A3-45AC-869A-B5DEB0369E8B}"/>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{7D9AB7E4-77FF-425E-B61B-10D8026EE552}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{C50B82D3-0DA4-4381-A87B-024540F50D43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -11645,32 +11695,32 @@
     <row r="1" spans="4:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="121" t="s">
+      <c r="E3" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="121" t="s">
+      <c r="F3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="123" t="s">
+      <c r="G3" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="124" t="s">
+      <c r="H3" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="126"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="118"/>
       <c r="N3" s="25"/>
     </row>
     <row r="4" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="120"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
       <c r="H4" s="76" t="s">
         <v>49</v>
       </c>
@@ -11732,10 +11782,10 @@
       <c r="L6" s="37"/>
     </row>
     <row r="7" spans="4:14" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="127" t="s">
+      <c r="D7" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="127" t="s">
+      <c r="E7" s="110" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="82" t="s">
@@ -11755,8 +11805,8 @@
       </c>
     </row>
     <row r="8" spans="4:14" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
       <c r="F8" s="82" t="s">
         <v>57</v>
       </c>
@@ -11774,8 +11824,8 @@
       </c>
     </row>
     <row r="9" spans="4:14" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
       <c r="F9" s="85" t="s">
         <v>68</v>
       </c>
@@ -11791,7 +11841,7 @@
       <c r="L9" s="41"/>
     </row>
     <row r="10" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="115" t="s">
+      <c r="D10" s="121" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="35" t="s">
@@ -11800,226 +11850,226 @@
       <c r="F10" s="78">
         <v>695000000</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="113" t="s">
+      <c r="H10" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
     </row>
     <row r="11" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="115"/>
+      <c r="D11" s="121"/>
       <c r="E11" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="33">
         <v>5000000</v>
       </c>
-      <c r="G11" s="117"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="113"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
     </row>
     <row r="12" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="115"/>
+      <c r="D12" s="121"/>
       <c r="E12" s="30" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="33">
         <v>2000000</v>
       </c>
-      <c r="G12" s="117"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
     </row>
     <row r="13" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="115"/>
+      <c r="D13" s="121"/>
       <c r="E13" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="33">
         <v>6000000</v>
       </c>
-      <c r="G13" s="117"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="119"/>
     </row>
     <row r="14" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="115"/>
+      <c r="D14" s="121"/>
       <c r="E14" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="33">
         <v>12000000</v>
       </c>
-      <c r="G14" s="117"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="119"/>
     </row>
     <row r="15" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="115"/>
+      <c r="D15" s="121"/>
       <c r="E15" s="30" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="33">
         <v>12000000</v>
       </c>
-      <c r="G15" s="117"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
     </row>
     <row r="16" spans="4:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="115"/>
+      <c r="D16" s="121"/>
       <c r="E16" s="30" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="33">
         <v>12000000</v>
       </c>
-      <c r="G16" s="117"/>
-      <c r="H16" s="113"/>
-      <c r="I16" s="113"/>
-      <c r="J16" s="113"/>
-      <c r="K16" s="113"/>
-      <c r="L16" s="113"/>
+      <c r="G16" s="123"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
     </row>
     <row r="17" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="115"/>
+      <c r="D17" s="121"/>
       <c r="E17" s="30" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="33">
         <v>4000000</v>
       </c>
-      <c r="G17" s="117"/>
-      <c r="H17" s="113"/>
-      <c r="I17" s="113"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
     </row>
     <row r="18" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="115"/>
+      <c r="D18" s="121"/>
       <c r="E18" s="30" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="33">
         <v>10000000</v>
       </c>
-      <c r="G18" s="117"/>
-      <c r="H18" s="113"/>
-      <c r="I18" s="113"/>
-      <c r="J18" s="113"/>
-      <c r="K18" s="113"/>
-      <c r="L18" s="113"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="119"/>
     </row>
     <row r="19" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="115"/>
+      <c r="D19" s="121"/>
       <c r="E19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="33">
         <v>480000000</v>
       </c>
-      <c r="G19" s="117"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
+      <c r="G19" s="123"/>
+      <c r="H19" s="119"/>
+      <c r="I19" s="119"/>
+      <c r="J19" s="119"/>
+      <c r="K19" s="119"/>
+      <c r="L19" s="119"/>
     </row>
     <row r="20" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="115"/>
+      <c r="D20" s="121"/>
       <c r="E20" s="30" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="33">
         <v>60000000</v>
       </c>
-      <c r="G20" s="117"/>
-      <c r="H20" s="113"/>
-      <c r="I20" s="113"/>
-      <c r="J20" s="113"/>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="119"/>
+      <c r="I20" s="119"/>
+      <c r="J20" s="119"/>
+      <c r="K20" s="119"/>
+      <c r="L20" s="119"/>
     </row>
     <row r="21" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="115"/>
+      <c r="D21" s="121"/>
       <c r="E21" s="30" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="33">
         <v>2000000</v>
       </c>
-      <c r="G21" s="117"/>
-      <c r="H21" s="113"/>
-      <c r="I21" s="113"/>
-      <c r="J21" s="113"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="113"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="119"/>
+      <c r="I21" s="119"/>
+      <c r="J21" s="119"/>
+      <c r="K21" s="119"/>
+      <c r="L21" s="119"/>
     </row>
     <row r="22" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="115"/>
+      <c r="D22" s="121"/>
       <c r="E22" s="30" t="s">
         <v>36</v>
       </c>
       <c r="F22" s="33">
         <v>5000000</v>
       </c>
-      <c r="G22" s="117"/>
-      <c r="H22" s="113"/>
-      <c r="I22" s="113"/>
-      <c r="J22" s="113"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="119"/>
     </row>
     <row r="23" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="115"/>
+      <c r="D23" s="121"/>
       <c r="E23" s="30" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="33">
         <v>25000000</v>
       </c>
-      <c r="G23" s="117"/>
-      <c r="H23" s="113"/>
-      <c r="I23" s="113"/>
-      <c r="J23" s="113"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="113"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
     </row>
     <row r="24" spans="4:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="116"/>
+      <c r="D24" s="122"/>
       <c r="E24" s="32" t="s">
         <v>38</v>
       </c>
       <c r="F24" s="33">
         <v>60000000</v>
       </c>
-      <c r="G24" s="118"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="114"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
     </row>
     <row r="25" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12999,20 +13049,20 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D10:D24"/>
+    <mergeCell ref="G10:G24"/>
+    <mergeCell ref="H10:H24"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="I10:I24"/>
     <mergeCell ref="J10:J24"/>
     <mergeCell ref="K10:K24"/>
     <mergeCell ref="L10:L24"/>
-    <mergeCell ref="D10:D24"/>
-    <mergeCell ref="G10:G24"/>
-    <mergeCell ref="H10:H24"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -13024,7 +13074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -13062,65 +13112,65 @@
       </c>
     </row>
     <row r="7" spans="3:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="128" t="s">
+      <c r="C7" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="138" t="s">
+      <c r="D7" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="140" t="s">
+      <c r="E7" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="142" t="s">
+      <c r="F7" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="144" t="s">
+      <c r="G7" s="141" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="129"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="136"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="144"/>
+      <c r="G8" s="133"/>
     </row>
     <row r="9" spans="3:7" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="129"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="137"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="134"/>
     </row>
     <row r="10" spans="3:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="128" t="s">
+      <c r="C10" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="138" t="s">
+      <c r="D10" s="135" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="140" t="s">
+      <c r="E10" s="137" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="142" t="s">
+      <c r="F10" s="139" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="144" t="s">
+      <c r="G10" s="141" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="130"/>
-      <c r="D11" s="139"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="143"/>
-      <c r="G11" s="136"/>
+      <c r="C11" s="127"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="138"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="133"/>
     </row>
     <row r="12" spans="3:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="131" t="s">
+      <c r="C12" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="149" t="s">
+      <c r="D12" s="146" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="47" t="s">
@@ -13134,8 +13184,8 @@
       </c>
     </row>
     <row r="13" spans="3:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="132"/>
-      <c r="D13" s="150"/>
+      <c r="C13" s="129"/>
+      <c r="D13" s="147"/>
       <c r="E13" s="50" t="s">
         <v>57</v>
       </c>
@@ -13147,8 +13197,8 @@
       </c>
     </row>
     <row r="14" spans="3:7" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="133"/>
-      <c r="D14" s="151"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="148"/>
       <c r="E14" s="52" t="s">
         <v>57</v>
       </c>
@@ -13160,7 +13210,7 @@
       </c>
     </row>
     <row r="15" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="134" t="s">
+      <c r="C15" s="131" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54" t="s">
@@ -13170,12 +13220,12 @@
       <c r="F15" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="136" t="s">
+      <c r="G15" s="133" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="134"/>
+      <c r="C16" s="131"/>
       <c r="D16" s="54" t="s">
         <v>25</v>
       </c>
@@ -13183,10 +13233,10 @@
       <c r="F16" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="136"/>
+      <c r="G16" s="133"/>
     </row>
     <row r="17" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="134"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="56" t="s">
         <v>26</v>
       </c>
@@ -13196,10 +13246,10 @@
       <c r="F17" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="136"/>
+      <c r="G17" s="133"/>
     </row>
     <row r="18" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="134"/>
+      <c r="C18" s="131"/>
       <c r="D18" s="56" t="s">
         <v>27</v>
       </c>
@@ -13209,10 +13259,10 @@
       <c r="F18" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="136"/>
+      <c r="G18" s="133"/>
     </row>
     <row r="19" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="134"/>
+      <c r="C19" s="131"/>
       <c r="D19" s="56" t="s">
         <v>28</v>
       </c>
@@ -13222,10 +13272,10 @@
       <c r="F19" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="136"/>
+      <c r="G19" s="133"/>
     </row>
     <row r="20" spans="3:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="134"/>
+      <c r="C20" s="131"/>
       <c r="D20" s="56" t="s">
         <v>29</v>
       </c>
@@ -13235,10 +13285,10 @@
       <c r="F20" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="136"/>
+      <c r="G20" s="133"/>
     </row>
     <row r="21" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="134"/>
+      <c r="C21" s="131"/>
       <c r="D21" s="56" t="s">
         <v>30</v>
       </c>
@@ -13248,10 +13298,10 @@
       <c r="F21" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="136"/>
+      <c r="G21" s="133"/>
     </row>
     <row r="22" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="134"/>
+      <c r="C22" s="131"/>
       <c r="D22" s="56" t="s">
         <v>31</v>
       </c>
@@ -13261,10 +13311,10 @@
       <c r="F22" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="136"/>
+      <c r="G22" s="133"/>
     </row>
     <row r="23" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="134"/>
+      <c r="C23" s="131"/>
       <c r="D23" s="54" t="s">
         <v>32</v>
       </c>
@@ -13274,10 +13324,10 @@
       <c r="F23" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="G23" s="136"/>
+      <c r="G23" s="133"/>
     </row>
     <row r="24" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="134"/>
+      <c r="C24" s="131"/>
       <c r="D24" s="54" t="s">
         <v>33</v>
       </c>
@@ -13287,10 +13337,10 @@
       <c r="F24" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="136"/>
+      <c r="G24" s="133"/>
     </row>
     <row r="25" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="134"/>
+      <c r="C25" s="131"/>
       <c r="D25" s="54" t="s">
         <v>34</v>
       </c>
@@ -13300,10 +13350,10 @@
       <c r="F25" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="136"/>
+      <c r="G25" s="133"/>
     </row>
     <row r="26" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="134"/>
+      <c r="C26" s="131"/>
       <c r="D26" s="54" t="s">
         <v>35</v>
       </c>
@@ -13313,10 +13363,10 @@
       <c r="F26" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="136"/>
+      <c r="G26" s="133"/>
     </row>
     <row r="27" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="134"/>
+      <c r="C27" s="131"/>
       <c r="D27" s="54" t="s">
         <v>36</v>
       </c>
@@ -13326,10 +13376,10 @@
       <c r="F27" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="136"/>
+      <c r="G27" s="133"/>
     </row>
     <row r="28" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="134"/>
+      <c r="C28" s="131"/>
       <c r="D28" s="54" t="s">
         <v>37</v>
       </c>
@@ -13339,10 +13389,10 @@
       <c r="F28" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="136"/>
+      <c r="G28" s="133"/>
     </row>
     <row r="29" spans="3:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="135"/>
+      <c r="C29" s="132"/>
       <c r="D29" s="59" t="s">
         <v>38</v>
       </c>
@@ -13352,7 +13402,7 @@
       <c r="F29" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="137"/>
+      <c r="G29" s="134"/>
     </row>
     <row r="30" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Apply corrections to supposed
</commit_message>
<xml_diff>
--- a/ExcelTables/Matrices para MML.xlsx
+++ b/ExcelTables/Matrices para MML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corra\OneDrive\Documentos\GitHub\AnalisisdeAlternativas\ExcelTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C993FDC-C9A2-4DAD-83B6-DCCD21B635D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A6D52-054B-483F-ACF4-C0CAFDDB1279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="145">
   <si>
     <t>NIVEL</t>
   </si>
@@ -549,6 +549,9 @@
   </si>
   <si>
     <t>Jefe de Área</t>
+  </si>
+  <si>
+    <t>Las entidades de tránsito entregan las APIs para garantizan la compatibilidad y operabilidad con los sistemas desarrollados.</t>
   </si>
 </sst>
 </file>
@@ -1792,6 +1795,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1803,15 +1815,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10014,27 +10017,27 @@
     <row r="2" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="107" t="s">
+      <c r="E4" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="107" t="s">
+      <c r="F4" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
     </row>
     <row r="5" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
       <c r="F5" s="64" t="s">
         <v>40</v>
       </c>
@@ -10052,10 +10055,10 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="105" t="s">
         <v>96</v>
       </c>
       <c r="E6" s="65"/>
@@ -10066,8 +10069,8 @@
       <c r="J6" s="65"/>
     </row>
     <row r="7" spans="3:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="108"/>
-      <c r="D7" s="109"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="105"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
       <c r="G7" s="65"/>
@@ -10076,8 +10079,8 @@
       <c r="J7" s="65"/>
     </row>
     <row r="8" spans="3:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
       <c r="E8" s="65"/>
       <c r="F8" s="66"/>
       <c r="G8" s="65"/>
@@ -10152,139 +10155,139 @@
       </c>
     </row>
     <row r="12" spans="3:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="106" t="s">
+      <c r="E12" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="103" t="s">
+      <c r="G12" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="H12" s="103" t="s">
+      <c r="H12" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="I12" s="103" t="s">
+      <c r="I12" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="J12" s="103" t="s">
+      <c r="J12" s="106" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="13" spans="3:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="105"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
     </row>
     <row r="14" spans="3:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="105"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="106"/>
+      <c r="J14" s="106"/>
     </row>
     <row r="15" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="105"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="103" t="s">
+      <c r="C15" s="108"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="103" t="s">
+      <c r="G15" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="103" t="s">
+      <c r="H15" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="103" t="s">
+      <c r="I15" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="106" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="16" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="105"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="106" t="s">
+      <c r="C16" s="108"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="106"/>
     </row>
     <row r="17" spans="3:10" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="105"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="103"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
     </row>
     <row r="18" spans="3:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="105"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="103" t="s">
+      <c r="C18" s="108"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="103" t="s">
+      <c r="G18" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="103" t="s">
+      <c r="H18" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="I18" s="103" t="s">
+      <c r="I18" s="106" t="s">
         <v>109</v>
       </c>
-      <c r="J18" s="103" t="s">
+      <c r="J18" s="106" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="19" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="105"/>
-      <c r="D19" s="103"/>
-      <c r="E19" s="106" t="s">
+      <c r="C19" s="108"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
     </row>
     <row r="20" spans="3:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="105"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="103"/>
-      <c r="I20" s="103"/>
-      <c r="J20" s="103"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="106"/>
     </row>
     <row r="21" spans="3:10" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="105"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="106"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="29" t="s">
         <v>82</v>
       </c>
@@ -10302,7 +10305,7 @@
       </c>
     </row>
     <row r="22" spans="3:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="104" t="s">
+      <c r="C22" s="107" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="71" t="s">
@@ -10328,7 +10331,7 @@
       </c>
     </row>
     <row r="23" spans="3:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="104"/>
+      <c r="C23" s="107"/>
       <c r="D23" s="71" t="s">
         <v>25</v>
       </c>
@@ -10352,7 +10355,7 @@
       </c>
     </row>
     <row r="24" spans="3:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="104"/>
+      <c r="C24" s="107"/>
       <c r="D24" s="29" t="s">
         <v>26</v>
       </c>
@@ -10376,7 +10379,7 @@
       </c>
     </row>
     <row r="25" spans="3:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="104"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="29" t="s">
         <v>27</v>
       </c>
@@ -10400,7 +10403,7 @@
       </c>
     </row>
     <row r="26" spans="3:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="104"/>
+      <c r="C26" s="107"/>
       <c r="D26" s="29" t="s">
         <v>28</v>
       </c>
@@ -10424,7 +10427,7 @@
       </c>
     </row>
     <row r="27" spans="3:10" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="104"/>
+      <c r="C27" s="107"/>
       <c r="D27" s="29" t="s">
         <v>29</v>
       </c>
@@ -10448,7 +10451,7 @@
       </c>
     </row>
     <row r="28" spans="3:10" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="104"/>
+      <c r="C28" s="107"/>
       <c r="D28" s="29" t="s">
         <v>30</v>
       </c>
@@ -10472,7 +10475,7 @@
       </c>
     </row>
     <row r="29" spans="3:10" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="104"/>
+      <c r="C29" s="107"/>
       <c r="D29" s="29" t="s">
         <v>31</v>
       </c>
@@ -10496,7 +10499,7 @@
       </c>
     </row>
     <row r="30" spans="3:10" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="104"/>
+      <c r="C30" s="107"/>
       <c r="D30" s="62" t="s">
         <v>32</v>
       </c>
@@ -10520,7 +10523,7 @@
       </c>
     </row>
     <row r="31" spans="3:10" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="104"/>
+      <c r="C31" s="107"/>
       <c r="D31" s="62" t="s">
         <v>33</v>
       </c>
@@ -10544,7 +10547,7 @@
       </c>
     </row>
     <row r="32" spans="3:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="104"/>
+      <c r="C32" s="107"/>
       <c r="D32" s="62" t="s">
         <v>34</v>
       </c>
@@ -10568,7 +10571,7 @@
       </c>
     </row>
     <row r="33" spans="3:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="104"/>
+      <c r="C33" s="107"/>
       <c r="D33" s="62" t="s">
         <v>35</v>
       </c>
@@ -10592,7 +10595,7 @@
       </c>
     </row>
     <row r="34" spans="3:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="104"/>
+      <c r="C34" s="107"/>
       <c r="D34" s="62" t="s">
         <v>36</v>
       </c>
@@ -10616,7 +10619,7 @@
       </c>
     </row>
     <row r="35" spans="3:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="104"/>
+      <c r="C35" s="107"/>
       <c r="D35" s="62" t="s">
         <v>37</v>
       </c>
@@ -10640,7 +10643,7 @@
       </c>
     </row>
     <row r="36" spans="3:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="104"/>
+      <c r="C36" s="107"/>
       <c r="D36" s="62" t="s">
         <v>38</v>
       </c>
@@ -11629,12 +11632,17 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="C22:C36"/>
+    <mergeCell ref="D12:D21"/>
+    <mergeCell ref="C12:C21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E12:E15"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="I15:I17"/>
@@ -11644,18 +11652,13 @@
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="I18:I20"/>
     <mergeCell ref="J18:J20"/>
-    <mergeCell ref="C22:C36"/>
-    <mergeCell ref="D12:D21"/>
-    <mergeCell ref="C12:C21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
     <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{7D9AB7E4-77FF-425E-B61B-10D8026EE552}"/>
@@ -11671,8 +11674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D1:N1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="E5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11786,7 +11789,7 @@
         <v>65</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="H7" s="84" t="s">
         <v>54</v>
@@ -13068,7 +13071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -13187,7 +13190,7 @@
         <v>79</v>
       </c>
       <c r="G13" s="49" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>